<commit_message>
added new files IO examples
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>AppUrl</t>
   </si>
@@ -33,9 +33,6 @@
     <t>test@gmail.com</t>
   </si>
   <si>
-    <t>pwd112233</t>
-  </si>
-  <si>
     <t>https://facebook.com</t>
   </si>
   <si>
@@ -58,13 +55,20 @@
   </si>
   <si>
     <t>tester</t>
+  </si>
+  <si>
+    <t>newPassword8877</t>
+  </si>
+  <si>
+    <t>mylatestpwd1122</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,14 +439,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -464,18 +468,18 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -502,22 +506,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -537,12 +541,12 @@
   <sheetData>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>